<commit_message>
linear regression draft 2
</commit_message>
<xml_diff>
--- a/src/data/test_data.xlsx
+++ b/src/data/test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdem\Documents\Project Files\CSCI_6221_V\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F837D4-534E-4287-950D-17A016CCB7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D46BE6C-74D9-4157-848C-858AACBAFE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="19416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,316 +40,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -357,207 +57,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -604,20 +118,20 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -645,31 +159,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -697,23 +194,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -725,168 +205,193 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:B546"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B551" sqref="B551"/>
+      <selection activeCell="A2" sqref="A2:A546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7420</v>
       </c>
@@ -894,7 +399,7 @@
         <v>13300000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8960</v>
       </c>
@@ -902,7 +407,7 @@
         <v>12250000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>9960</v>
       </c>
@@ -910,7 +415,7 @@
         <v>12250000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7500</v>
       </c>
@@ -918,7 +423,7 @@
         <v>12215000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>7420</v>
       </c>

</xml_diff>

<commit_message>
linear regression v2 - complete
</commit_message>
<xml_diff>
--- a/src/data/test_data.xlsx
+++ b/src/data/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdem\Documents\Project Files\CSCI_6221_V\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE562D4-9FF0-4C01-AF7C-8D4DEE1DB994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078D4168-4166-4850-9841-4A9AD52C260F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="19416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,7 +882,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>350</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -912,7 +912,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -920,7 +920,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -928,7 +928,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -936,7 +936,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>750</v>
+        <v>755</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>850</v>
+        <v>856</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -952,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>950</v>
+        <v>957</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>1050</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -968,7 +968,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>1150</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -976,7 +976,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>1250</v>
+        <v>1060</v>
       </c>
     </row>
   </sheetData>

</xml_diff>